<commit_message>
7 screens-refunds,asset,contract,entitlement,product,returnorder,alternativepayment,changes in catch block message
</commit_message>
<xml_diff>
--- a/src/test/resources/sales_data.xlsx
+++ b/src/test/resources/sales_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhilashBysani-Kairo\eclipse-workspace\KITAP\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69623C8F-EE0A-4139-9128-A7930925A1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0513A2-92D2-4471-A48C-1AAB282AB658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1154">
   <si>
     <t>TCID</t>
   </si>
@@ -5193,8 +5193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B2B285-2FF8-4C37-B237-455EB8E487AB}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,8 +5290,8 @@
       <c r="D2" s="32" t="s">
         <v>542</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>543</v>
+      <c r="E2" s="65" t="s">
+        <v>252</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>544</v>
@@ -5408,8 +5408,8 @@
       <c r="D4" s="32" t="s">
         <v>507</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>543</v>
+      <c r="E4" s="65" t="s">
+        <v>252</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>569</v>
@@ -5467,7 +5467,7 @@
       <c r="D5" s="32" t="s">
         <v>542</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="65" t="s">
         <v>252</v>
       </c>
       <c r="F5" s="33" t="s">
@@ -5531,7 +5531,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I5"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10675,7 +10675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FA6DB-7D08-4418-AABC-61453176D845}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -11300,9 +11300,9 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0431C58D-B94F-41D2-BB24-AD8F80490DDE}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -11320,7 +11320,7 @@
     <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -11357,8 +11357,11 @@
       <c r="L1" s="6" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="6" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>317</v>
       </c>
@@ -11395,8 +11398,11 @@
       <c r="L2" s="5" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>317</v>
       </c>
@@ -11433,8 +11439,11 @@
       <c r="L3" s="5" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>317</v>
       </c>
@@ -11471,8 +11480,11 @@
       <c r="L4" s="5" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="65" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>317</v>
       </c>
@@ -11508,6 +11520,9 @@
       </c>
       <c r="L5" s="5" t="s">
         <v>298</v>
+      </c>
+      <c r="M5" s="65" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in pom.xml file and also added listeners class in utilities package
</commit_message>
<xml_diff>
--- a/src/test/resources/sales_data.xlsx
+++ b/src/test/resources/sales_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhilashBysani-Kairo\eclipse-workspace\KITAP\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34564AB-2DDA-411C-B196-26B1E7078DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284F83CF-6A11-4280-B4AE-865A6AB845C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="32" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="24" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -39,18 +39,19 @@
     <sheet name="RefundCreationViaUI" sheetId="12" r:id="rId24"/>
     <sheet name="PaymentCreationViaUI" sheetId="17" r:id="rId25"/>
     <sheet name="ContactsCreationViaUI" sheetId="5" r:id="rId26"/>
-    <sheet name="OrderCreationViaUI" sheetId="19" r:id="rId27"/>
-    <sheet name="LeadCreation" sheetId="7" r:id="rId28"/>
-    <sheet name="CasesCreationViaUI" sheetId="8" r:id="rId29"/>
-    <sheet name="ContractsCreationViaUI" sheetId="15" r:id="rId30"/>
-    <sheet name="AssetCreationViaUI" sheetId="16" r:id="rId31"/>
-    <sheet name="ProductCreationViaUI" sheetId="20" r:id="rId32"/>
-    <sheet name="CampaignCreationViaUI" sheetId="23" r:id="rId33"/>
-    <sheet name="ServiceAppointmentCreationViaUI" sheetId="27" r:id="rId34"/>
-    <sheet name="CardPaymentMethodCreationViaUI" sheetId="35" r:id="rId35"/>
-    <sheet name="ChangeRequestCreationViaUI" sheetId="28" r:id="rId36"/>
-    <sheet name="QuickTextCreationViaUI" sheetId="29" r:id="rId37"/>
-    <sheet name="BankingManagementCreationViaUI" sheetId="34" r:id="rId38"/>
+    <sheet name="sampletestclass" sheetId="46" r:id="rId27"/>
+    <sheet name="OrderCreationViaUI" sheetId="19" r:id="rId28"/>
+    <sheet name="LeadCreation" sheetId="7" r:id="rId29"/>
+    <sheet name="CasesCreationViaUI" sheetId="8" r:id="rId30"/>
+    <sheet name="ContractsCreationViaUI" sheetId="15" r:id="rId31"/>
+    <sheet name="AssetCreationViaUI" sheetId="16" r:id="rId32"/>
+    <sheet name="ProductCreationViaUI" sheetId="20" r:id="rId33"/>
+    <sheet name="CampaignCreationViaUI" sheetId="23" r:id="rId34"/>
+    <sheet name="ServiceAppointmentCreationViaUI" sheetId="27" r:id="rId35"/>
+    <sheet name="CardPaymentMethodCreationViaUI" sheetId="35" r:id="rId36"/>
+    <sheet name="ChangeRequestCreationViaUI" sheetId="28" r:id="rId37"/>
+    <sheet name="QuickTextCreationViaUI" sheetId="29" r:id="rId38"/>
+    <sheet name="BankingManagementCreationViaUI" sheetId="34" r:id="rId39"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="1195">
   <si>
     <t>TCID</t>
   </si>
@@ -3641,6 +3642,12 @@
   </si>
   <si>
     <t>1440</t>
+  </si>
+  <si>
+    <t>AccountListPageClassic</t>
+  </si>
+  <si>
+    <t>sampletestclass</t>
   </si>
 </sst>
 </file>
@@ -4296,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,10 +4611,26 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="92" t="s">
         <v>1164</v>
       </c>
       <c r="B38" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="92" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B39" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B40" s="69" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7077,7 +7100,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="92" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="91" t="s">
         <v>1130</v>
       </c>
@@ -7179,7 +7202,7 @@
       </c>
       <c r="Q13" s="72"/>
     </row>
-    <row r="14" spans="1:17" s="92" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="91" t="s">
         <v>1130</v>
       </c>
@@ -9841,6 +9864,363 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF1CF74-FF37-4005-B4CF-29C75DFBEF5B}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>625</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>626</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>627</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>628</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>629</v>
+      </c>
+      <c r="K1" s="67" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" s="67" t="s">
+        <v>656</v>
+      </c>
+      <c r="N1" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" s="67" t="s">
+        <v>657</v>
+      </c>
+      <c r="P1" s="67" t="s">
+        <v>658</v>
+      </c>
+      <c r="Q1" s="67" t="s">
+        <v>659</v>
+      </c>
+      <c r="R1" s="67" t="s">
+        <v>660</v>
+      </c>
+      <c r="S1" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="67" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>630</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>631</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>632</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>633</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>634</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="J2" s="65" t="s">
+        <v>637</v>
+      </c>
+      <c r="K2" s="65" t="s">
+        <v>661</v>
+      </c>
+      <c r="L2" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" s="65" t="s">
+        <v>535</v>
+      </c>
+      <c r="N2" s="65" t="s">
+        <v>665</v>
+      </c>
+      <c r="O2" s="65" t="s">
+        <v>669</v>
+      </c>
+      <c r="P2" s="65" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q2" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="R2" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="S2" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2" s="65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>639</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>640</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>641</v>
+      </c>
+      <c r="G3" s="66" t="s">
+        <v>642</v>
+      </c>
+      <c r="H3" s="65" t="s">
+        <v>643</v>
+      </c>
+      <c r="I3" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="J3" s="65" t="s">
+        <v>637</v>
+      </c>
+      <c r="K3" s="65" t="s">
+        <v>662</v>
+      </c>
+      <c r="L3" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="M3" s="65" t="s">
+        <v>664</v>
+      </c>
+      <c r="N3" s="65" t="s">
+        <v>666</v>
+      </c>
+      <c r="O3" s="65" t="s">
+        <v>670</v>
+      </c>
+      <c r="P3" s="65" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q3" s="65" t="s">
+        <v>406</v>
+      </c>
+      <c r="R3" s="65" t="s">
+        <v>406</v>
+      </c>
+      <c r="S3" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="T3" s="65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>645</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>646</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>647</v>
+      </c>
+      <c r="G4" s="66" t="s">
+        <v>648</v>
+      </c>
+      <c r="H4" s="65" t="s">
+        <v>649</v>
+      </c>
+      <c r="I4" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="J4" s="65" t="s">
+        <v>637</v>
+      </c>
+      <c r="K4" s="65" t="s">
+        <v>663</v>
+      </c>
+      <c r="L4" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="M4" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="65" t="s">
+        <v>667</v>
+      </c>
+      <c r="O4" s="65" t="s">
+        <v>671</v>
+      </c>
+      <c r="P4" s="65" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q4" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="R4" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="S4" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="T4" s="65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>650</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>651</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>652</v>
+      </c>
+      <c r="F5" s="66" t="s">
+        <v>653</v>
+      </c>
+      <c r="G5" s="66" t="s">
+        <v>654</v>
+      </c>
+      <c r="H5" s="65" t="s">
+        <v>655</v>
+      </c>
+      <c r="I5" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>637</v>
+      </c>
+      <c r="K5" s="65" t="s">
+        <v>663</v>
+      </c>
+      <c r="L5" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="M5" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="N5" s="65" t="s">
+        <v>668</v>
+      </c>
+      <c r="O5" s="65" t="s">
+        <v>671</v>
+      </c>
+      <c r="P5" s="65" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q5" s="65" t="s">
+        <v>406</v>
+      </c>
+      <c r="R5" s="65" t="s">
+        <v>406</v>
+      </c>
+      <c r="S5" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="T5" s="65" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7BF83388-87F1-4AE5-893F-B80C112E1404}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="test@test1.com" xr:uid="{16AF2239-8CF0-4406-BD5F-17632C1B470F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B83D26E-E4B1-4F7E-B100-64FB3E1B7752}">
   <dimension ref="A1:R5"/>
   <sheetViews>
@@ -10156,7 +10536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC57CCD-E72C-4B9C-834A-E37CEA5B08CD}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -10604,352 +10984,6 @@
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{86032F1D-6722-4981-BE64-F0E693A89E01}"/>
     <hyperlink ref="I3:I5" r:id="rId2" display="test@salesforce.com" xr:uid="{DAE28224-90F9-4100-A00F-A933840B5F92}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819E0DFE-C3E3-43E2-9AF5-23D7275B0D5A}">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>624</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>625</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>626</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>627</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>628</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>629</v>
-      </c>
-      <c r="K1" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>656</v>
-      </c>
-      <c r="N1" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="O1" s="34" t="s">
-        <v>657</v>
-      </c>
-      <c r="P1" s="34" t="s">
-        <v>658</v>
-      </c>
-      <c r="Q1" s="34" t="s">
-        <v>659</v>
-      </c>
-      <c r="R1" s="34" t="s">
-        <v>660</v>
-      </c>
-      <c r="S1" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>630</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>631</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>632</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>634</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>635</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>636</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>661</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>665</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>669</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>672</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>638</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>640</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>641</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>642</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>643</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>636</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>662</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>664</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>666</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>670</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>673</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="R3" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="S3" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="T3" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>644</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>645</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>646</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>647</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>648</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>649</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>636</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>663</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>667</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>671</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>674</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="R4" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="T4" s="32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>650</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>651</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>653</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>654</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>655</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>636</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>663</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="M5" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>668</v>
-      </c>
-      <c r="O5" s="32" t="s">
-        <v>671</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="S5" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{97F4D6FC-7A82-4B45-B6FF-12B0A5638E5C}"/>
-    <hyperlink ref="C3:C5" r:id="rId2" display="test@test1.com" xr:uid="{CB94EDDB-33AD-496C-A1BB-C5E470C07626}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11096,6 +11130,352 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819E0DFE-C3E3-43E2-9AF5-23D7275B0D5A}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>625</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>626</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>627</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>628</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>629</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>656</v>
+      </c>
+      <c r="N1" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>657</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>658</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>659</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>660</v>
+      </c>
+      <c r="S1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>630</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>631</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>632</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>634</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>661</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>535</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>665</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>669</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="S2" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>639</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>640</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>641</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>642</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>643</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>662</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>664</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>666</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>670</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>645</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>646</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>647</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>663</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>667</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>671</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="R4" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="S4" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>650</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>651</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>653</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>654</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>655</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>663</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>668</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>671</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="S5" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="T5" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{97F4D6FC-7A82-4B45-B6FF-12B0A5638E5C}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="test@test1.com" xr:uid="{CB94EDDB-33AD-496C-A1BB-C5E470C07626}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49992A8C-CEDE-44B4-A5C0-14F595B92F38}">
   <dimension ref="A1:S5"/>
   <sheetViews>
@@ -11426,7 +11806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0431C58D-B94F-41D2-BB24-AD8F80490DDE}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -11660,7 +12040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A93AEF-AC4C-4E43-8298-74EC462A1CCF}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -11768,7 +12148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD09B47-F8E2-4ADB-BC05-907EE49357C3}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -12003,11 +12383,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB7298-BA6C-497A-A2B3-9B7A9AB9A36C}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4:L5"/>
     </sheetView>
   </sheetViews>
@@ -12468,7 +12848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72C92E1-0035-4885-912A-76C73D1357BA}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -12926,7 +13306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60D7E1E-778D-4D47-B19A-27F68604DB84}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -13058,7 +13438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4341CDA3-B217-4AD7-90F1-223EDA293136}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -13166,7 +13546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C277418-5178-4E09-B036-AC53F9C98B37}">
   <dimension ref="A1:P5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Web & Mobile Standard framework
</commit_message>
<xml_diff>
--- a/src/test/resources/sales_data.xlsx
+++ b/src/test/resources/sales_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhilashBysani-Kairo\eclipse-workspace\KITAP\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9FAD51-C397-4D67-8D51-549737A22559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FF467B-9017-4287-B948-76551DC8F43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="29" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3267" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="1318">
   <si>
     <t>TCID</t>
   </si>
@@ -4008,16 +4008,19 @@
     <t>casenumber</t>
   </si>
   <si>
-    <t xml:space="preserve">      01270491              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      01270492              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      01270493              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      01270499              </t>
+    <t>Not Submitted</t>
+  </si>
+  <si>
+    <t>SzF0YXBEZW1v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      01270560              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      01270562              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      01270563              </t>
   </si>
 </sst>
 </file>
@@ -4025,7 +4028,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4162,8 +4165,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4191,6 +4200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4251,7 +4266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -4436,12 +4451,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6116,12 +6138,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId19" xr:uid="{F9295186-7613-4C75-816B-F48146E39E8F}"/>
-    <hyperlink ref="C3" r:id="rId20" xr:uid="{9EBC1A17-46DD-4C50-9F0D-9CE62CBC1089}"/>
-    <hyperlink ref="C4" r:id="rId21" xr:uid="{1FDCD2C8-6947-4DB7-B958-18A769211108}"/>
-    <hyperlink ref="C5" r:id="rId22" xr:uid="{2054EA05-D121-44A5-A503-957D55AA393B}"/>
-    <hyperlink ref="R2" r:id="rId23" xr:uid="{F7F09851-DDDF-435B-9236-3AC8D13F173E}"/>
-    <hyperlink ref="R3:R5" r:id="rId24" display="audit@kairos.com" xr:uid="{95C01D92-6365-4AB2-8110-8780301B2BF1}"/>
+    <hyperlink ref="C2" r:id="rId13" xr:uid="{F9295186-7613-4C75-816B-F48146E39E8F}"/>
+    <hyperlink ref="C3" r:id="rId14" xr:uid="{9EBC1A17-46DD-4C50-9F0D-9CE62CBC1089}"/>
+    <hyperlink ref="C4" r:id="rId15" xr:uid="{1FDCD2C8-6947-4DB7-B958-18A769211108}"/>
+    <hyperlink ref="C5" r:id="rId16" xr:uid="{2054EA05-D121-44A5-A503-957D55AA393B}"/>
+    <hyperlink ref="R2" r:id="rId17" xr:uid="{F7F09851-DDDF-435B-9236-3AC8D13F173E}"/>
+    <hyperlink ref="R3:R5" r:id="rId18" display="audit@kairos.com" xr:uid="{95C01D92-6365-4AB2-8110-8780301B2BF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7707,9 +7729,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I12" r:id="rId10" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{2235D1FA-55DF-475F-BBAF-85697A7EFF54}"/>
-    <hyperlink ref="I13" r:id="rId11" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{52E4FBF3-D500-46C8-8B9C-1300A73F614D}"/>
-    <hyperlink ref="I14" r:id="rId12" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{C6566594-5261-4F94-9F13-1E10AF9635C7}"/>
+    <hyperlink ref="I12" r:id="rId7" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{2235D1FA-55DF-475F-BBAF-85697A7EFF54}"/>
+    <hyperlink ref="I13" r:id="rId8" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{52E4FBF3-D500-46C8-8B9C-1300A73F614D}"/>
+    <hyperlink ref="I14" r:id="rId9" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{C6566594-5261-4F94-9F13-1E10AF9635C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9117,7 +9139,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId5" xr:uid="{0A0B9B83-5E3F-409B-B178-56F413CF49CD}"/>
+    <hyperlink ref="T2" r:id="rId4" xr:uid="{0A0B9B83-5E3F-409B-B178-56F413CF49CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10059,16 +10081,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId31" xr:uid="{9AA48684-DB5B-47C3-B8AF-5E6D91169907}"/>
-    <hyperlink ref="T3" r:id="rId32" xr:uid="{BF84467E-B7BA-4B3A-A065-8D675C45C212}"/>
-    <hyperlink ref="T4" r:id="rId33" xr:uid="{8DE751D3-C5E8-4D3D-98E4-8BEED21693C9}"/>
-    <hyperlink ref="T5" r:id="rId34" xr:uid="{FD91436E-F8E2-43E4-85EA-1FE77DB03927}"/>
-    <hyperlink ref="I18" r:id="rId35" xr:uid="{E1324038-61D0-4F0C-9802-52D709AB3ED7}"/>
-    <hyperlink ref="I19" r:id="rId36" xr:uid="{416467B9-F05B-45CE-BBF7-59BF1E292E46}"/>
-    <hyperlink ref="I20" r:id="rId37" xr:uid="{CDBC7271-9477-4D8C-9241-8D7A074BC3D8}"/>
-    <hyperlink ref="T26" r:id="rId38" xr:uid="{FDE20BFB-9FEB-4A83-ABE0-1FDFE45393BC}"/>
-    <hyperlink ref="T27" r:id="rId39" xr:uid="{B053766D-1E88-41FC-88A9-3799AB16E4D2}"/>
-    <hyperlink ref="T28" r:id="rId40" xr:uid="{FFAD2A89-41FE-4FC0-923D-7FB8BEB1E54D}"/>
+    <hyperlink ref="T2" r:id="rId21" xr:uid="{9AA48684-DB5B-47C3-B8AF-5E6D91169907}"/>
+    <hyperlink ref="T3" r:id="rId22" xr:uid="{BF84467E-B7BA-4B3A-A065-8D675C45C212}"/>
+    <hyperlink ref="T4" r:id="rId23" xr:uid="{8DE751D3-C5E8-4D3D-98E4-8BEED21693C9}"/>
+    <hyperlink ref="T5" r:id="rId24" xr:uid="{FD91436E-F8E2-43E4-85EA-1FE77DB03927}"/>
+    <hyperlink ref="I18" r:id="rId25" xr:uid="{E1324038-61D0-4F0C-9802-52D709AB3ED7}"/>
+    <hyperlink ref="I19" r:id="rId26" xr:uid="{416467B9-F05B-45CE-BBF7-59BF1E292E46}"/>
+    <hyperlink ref="I20" r:id="rId27" xr:uid="{CDBC7271-9477-4D8C-9241-8D7A074BC3D8}"/>
+    <hyperlink ref="T26" r:id="rId28" xr:uid="{FDE20BFB-9FEB-4A83-ABE0-1FDFE45393BC}"/>
+    <hyperlink ref="T27" r:id="rId29" xr:uid="{B053766D-1E88-41FC-88A9-3799AB16E4D2}"/>
+    <hyperlink ref="T28" r:id="rId30" xr:uid="{FFAD2A89-41FE-4FC0-923D-7FB8BEB1E54D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10308,7 +10330,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId5" xr:uid="{542370F0-976D-423C-94B6-9AF16B6988FC}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{542370F0-976D-423C-94B6-9AF16B6988FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10665,8 +10687,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId7" xr:uid="{7BF83388-87F1-4AE5-893F-B80C112E1404}"/>
-    <hyperlink ref="C3:C5" r:id="rId8" display="test@test1.com" xr:uid="{16AF2239-8CF0-4406-BD5F-17632C1B470F}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{7BF83388-87F1-4AE5-893F-B80C112E1404}"/>
+    <hyperlink ref="C3:C5" r:id="rId6" display="test@test1.com" xr:uid="{16AF2239-8CF0-4406-BD5F-17632C1B470F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11234,7 +11256,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I20:I22" r:id="rId4" display="test@salesforce.com" xr:uid="{A44EB65D-397D-47E2-9929-1D7B8E65774B}"/>
+    <hyperlink ref="I20:I22" r:id="rId3" display="test@salesforce.com" xr:uid="{A44EB65D-397D-47E2-9929-1D7B8E65774B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11437,7 +11459,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId4" xr:uid="{86032F1D-6722-4981-BE64-F0E693A89E01}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{86032F1D-6722-4981-BE64-F0E693A89E01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11588,9 +11610,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId11" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{472E020E-B502-4DFC-B016-5A6103264EEC}"/>
-    <hyperlink ref="R2" r:id="rId12" xr:uid="{B8CE6728-8681-40EC-9ED4-2A5DA6683852}"/>
-    <hyperlink ref="Q2" r:id="rId13" xr:uid="{E7AEBF32-8D0E-4499-A6FB-CC997BC5FA39}"/>
+    <hyperlink ref="I2" r:id="rId8" tooltip="mailto:surya@gmail.com" display="mailto:surya@gmail.com" xr:uid="{472E020E-B502-4DFC-B016-5A6103264EEC}"/>
+    <hyperlink ref="R2" r:id="rId9" xr:uid="{B8CE6728-8681-40EC-9ED4-2A5DA6683852}"/>
+    <hyperlink ref="Q2" r:id="rId10" xr:uid="{E7AEBF32-8D0E-4499-A6FB-CC997BC5FA39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -11601,8 +11623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B86C09-C398-4434-95BA-ADB1923B7409}">
   <dimension ref="A1:CV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="CM1" workbookViewId="0">
+      <selection activeCell="CU2" sqref="CU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11610,8 +11632,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" style="62" width="14.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="62" width="13.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="62" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="62" width="15.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="62" width="15.140625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="62" width="15.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="62" width="13.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="62" width="12.0" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="62" width="11.0" collapsed="true"/>
@@ -11699,309 +11720,309 @@
     <col min="101" max="16384" style="62" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="89" customFormat="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:100" s="105" customFormat="1">
+      <c r="A1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="105" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="105" t="s">
         <v>1312</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="105" t="s">
         <v>479</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="105" t="s">
         <v>621</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="105" t="s">
         <v>622</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="105" t="s">
         <v>623</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="105" t="s">
         <v>624</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="105" t="s">
         <v>625</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="N1" s="89" t="s">
+      <c r="N1" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="O1" s="89" t="s">
+      <c r="O1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="P1" s="89" t="s">
+      <c r="P1" s="105" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="105" t="s">
         <v>653</v>
       </c>
-      <c r="R1" s="89" t="s">
+      <c r="R1" s="105" t="s">
         <v>654</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="105" t="s">
         <v>655</v>
       </c>
-      <c r="T1" s="89" t="s">
+      <c r="T1" s="105" t="s">
         <v>656</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="89" t="s">
+      <c r="V1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="89" t="s">
+      <c r="W1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="X1" s="89" t="s">
+      <c r="X1" s="105" t="s">
         <v>1199</v>
       </c>
-      <c r="Y1" s="89" t="s">
+      <c r="Y1" s="105" t="s">
         <v>1209</v>
       </c>
-      <c r="Z1" s="89" t="s">
+      <c r="Z1" s="105" t="s">
         <v>1210</v>
       </c>
-      <c r="AA1" s="89" t="s">
+      <c r="AA1" s="105" t="s">
         <v>1211</v>
       </c>
-      <c r="AB1" s="89" t="s">
+      <c r="AB1" s="105" t="s">
         <v>796</v>
       </c>
-      <c r="AC1" s="89" t="s">
+      <c r="AC1" s="105" t="s">
         <v>1212</v>
       </c>
-      <c r="AD1" s="89" t="s">
+      <c r="AD1" s="105" t="s">
         <v>1213</v>
       </c>
-      <c r="AE1" s="89" t="s">
+      <c r="AE1" s="105" t="s">
         <v>1214</v>
       </c>
-      <c r="AF1" s="89" t="s">
+      <c r="AF1" s="105" t="s">
         <v>1215</v>
       </c>
-      <c r="AG1" s="89" t="s">
+      <c r="AG1" s="105" t="s">
         <v>1216</v>
       </c>
-      <c r="AH1" s="89" t="s">
+      <c r="AH1" s="105" t="s">
         <v>1217</v>
       </c>
-      <c r="AI1" s="89" t="s">
+      <c r="AI1" s="105" t="s">
         <v>1218</v>
       </c>
-      <c r="AJ1" s="89" t="s">
+      <c r="AJ1" s="105" t="s">
         <v>1219</v>
       </c>
-      <c r="AK1" s="89" t="s">
+      <c r="AK1" s="105" t="s">
         <v>1220</v>
       </c>
-      <c r="AL1" s="89" t="s">
+      <c r="AL1" s="105" t="s">
         <v>1221</v>
       </c>
-      <c r="AM1" s="89" t="s">
+      <c r="AM1" s="105" t="s">
         <v>1222</v>
       </c>
       <c r="AN1" s="106" t="s">
         <v>1299</v>
       </c>
-      <c r="AO1" s="89" t="s">
+      <c r="AO1" s="105" t="s">
         <v>1223</v>
       </c>
-      <c r="AP1" s="89" t="s">
+      <c r="AP1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="AQ1" s="89" t="s">
+      <c r="AQ1" s="105" t="s">
         <v>1224</v>
       </c>
-      <c r="AR1" s="89" t="s">
+      <c r="AR1" s="105" t="s">
         <v>1302</v>
       </c>
-      <c r="AS1" s="89" t="s">
+      <c r="AS1" s="105" t="s">
         <v>479</v>
       </c>
-      <c r="AT1" s="89" t="s">
+      <c r="AT1" s="105" t="s">
         <v>1225</v>
       </c>
-      <c r="AU1" s="89" t="s">
+      <c r="AU1" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="AV1" s="89" t="s">
+      <c r="AV1" s="105" t="s">
         <v>1304</v>
       </c>
-      <c r="AW1" s="89" t="s">
+      <c r="AW1" s="105" t="s">
         <v>1227</v>
       </c>
-      <c r="AX1" s="89" t="s">
+      <c r="AX1" s="105" t="s">
         <v>1228</v>
       </c>
-      <c r="AY1" s="89" t="s">
+      <c r="AY1" s="105" t="s">
         <v>1229</v>
       </c>
-      <c r="AZ1" s="89" t="s">
+      <c r="AZ1" s="105" t="s">
         <v>1230</v>
       </c>
-      <c r="BA1" s="89" t="s">
+      <c r="BA1" s="105" t="s">
         <v>1231</v>
       </c>
-      <c r="BB1" s="89" t="s">
+      <c r="BB1" s="105" t="s">
         <v>1232</v>
       </c>
-      <c r="BC1" s="89" t="s">
+      <c r="BC1" s="105" t="s">
         <v>1233</v>
       </c>
-      <c r="BD1" s="89" t="s">
+      <c r="BD1" s="105" t="s">
         <v>1234</v>
       </c>
-      <c r="BE1" s="89" t="s">
+      <c r="BE1" s="105" t="s">
         <v>1235</v>
       </c>
-      <c r="BF1" s="89" t="s">
+      <c r="BF1" s="105" t="s">
         <v>1236</v>
       </c>
-      <c r="BG1" s="89" t="s">
+      <c r="BG1" s="105" t="s">
         <v>1237</v>
       </c>
-      <c r="BH1" s="89" t="s">
+      <c r="BH1" s="105" t="s">
         <v>1238</v>
       </c>
-      <c r="BI1" s="89" t="s">
+      <c r="BI1" s="105" t="s">
         <v>1239</v>
       </c>
-      <c r="BJ1" s="89" t="s">
+      <c r="BJ1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BK1" s="89" t="s">
+      <c r="BK1" s="105" t="s">
         <v>1241</v>
       </c>
-      <c r="BL1" s="89" t="s">
+      <c r="BL1" s="105" t="s">
         <v>1242</v>
       </c>
-      <c r="BM1" s="89" t="s">
+      <c r="BM1" s="105" t="s">
         <v>1243</v>
       </c>
-      <c r="BN1" s="89" t="s">
+      <c r="BN1" s="105" t="s">
         <v>1244</v>
       </c>
-      <c r="BO1" s="89" t="s">
+      <c r="BO1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BP1" s="89" t="s">
+      <c r="BP1" s="105" t="s">
         <v>1245</v>
       </c>
-      <c r="BQ1" s="89" t="s">
+      <c r="BQ1" s="105" t="s">
         <v>1246</v>
       </c>
-      <c r="BR1" s="89" t="s">
+      <c r="BR1" s="105" t="s">
         <v>1247</v>
       </c>
-      <c r="BS1" s="89" t="s">
+      <c r="BS1" s="105" t="s">
         <v>1248</v>
       </c>
-      <c r="BT1" s="89" t="s">
+      <c r="BT1" s="105" t="s">
         <v>1249</v>
       </c>
-      <c r="BU1" s="89" t="s">
+      <c r="BU1" s="105" t="s">
         <v>1250</v>
       </c>
-      <c r="BV1" s="89" t="s">
+      <c r="BV1" s="105" t="s">
         <v>1251</v>
       </c>
-      <c r="BW1" s="89" t="s">
+      <c r="BW1" s="105" t="s">
         <v>1252</v>
       </c>
-      <c r="BX1" s="89" t="s">
+      <c r="BX1" s="105" t="s">
         <v>1253</v>
       </c>
-      <c r="BY1" s="89" t="s">
+      <c r="BY1" s="105" t="s">
         <v>1254</v>
       </c>
-      <c r="BZ1" s="89" t="s">
+      <c r="BZ1" s="105" t="s">
         <v>1255</v>
       </c>
-      <c r="CA1" s="89" t="s">
+      <c r="CA1" s="105" t="s">
         <v>1256</v>
       </c>
-      <c r="CB1" s="89" t="s">
+      <c r="CB1" s="105" t="s">
         <v>1257</v>
       </c>
-      <c r="CC1" s="89" t="s">
+      <c r="CC1" s="105" t="s">
         <v>1258</v>
       </c>
-      <c r="CD1" s="89" t="s">
+      <c r="CD1" s="105" t="s">
         <v>1259</v>
       </c>
-      <c r="CE1" s="89" t="s">
+      <c r="CE1" s="105" t="s">
         <v>1260</v>
       </c>
-      <c r="CF1" s="89" t="s">
+      <c r="CF1" s="105" t="s">
         <v>1310</v>
       </c>
-      <c r="CG1" s="89" t="s">
+      <c r="CG1" s="105" t="s">
         <v>1262</v>
       </c>
-      <c r="CH1" s="89" t="s">
+      <c r="CH1" s="105" t="s">
         <v>1263</v>
       </c>
-      <c r="CI1" s="89" t="s">
+      <c r="CI1" s="105" t="s">
         <v>1264</v>
       </c>
-      <c r="CJ1" s="89" t="s">
+      <c r="CJ1" s="105" t="s">
         <v>1265</v>
       </c>
-      <c r="CK1" s="89" t="s">
+      <c r="CK1" s="105" t="s">
         <v>1266</v>
       </c>
-      <c r="CL1" s="89" t="s">
+      <c r="CL1" s="105" t="s">
         <v>1267</v>
       </c>
-      <c r="CM1" s="89" t="s">
+      <c r="CM1" s="105" t="s">
         <v>1268</v>
       </c>
-      <c r="CN1" s="89" t="s">
+      <c r="CN1" s="105" t="s">
         <v>1269</v>
       </c>
-      <c r="CO1" s="89" t="s">
+      <c r="CO1" s="105" t="s">
         <v>1270</v>
       </c>
-      <c r="CP1" s="89" t="s">
+      <c r="CP1" s="105" t="s">
         <v>1271</v>
       </c>
-      <c r="CQ1" s="89" t="s">
+      <c r="CQ1" s="105" t="s">
         <v>1272</v>
       </c>
-      <c r="CR1" s="89" t="s">
+      <c r="CR1" s="105" t="s">
         <v>1273</v>
       </c>
-      <c r="CS1" s="89" t="s">
+      <c r="CS1" s="105" t="s">
         <v>1274</v>
       </c>
-      <c r="CT1" s="102" t="s">
+      <c r="CT1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="CU1" s="102" t="s">
+      <c r="CU1" s="105" t="s">
         <v>1199</v>
       </c>
-      <c r="CV1" s="89" t="s">
+      <c r="CV1" s="105" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="2" spans="1:100" s="89" customFormat="1">
+    <row r="2" spans="1:100" s="89" customFormat="1" ht="16.5">
       <c r="A2" s="89" t="s">
         <v>21</v>
       </c>
@@ -12012,7 +12033,7 @@
         <v>626</v>
       </c>
       <c r="D2" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>511</v>
@@ -12125,16 +12146,16 @@
       <c r="AO2" s="89" t="s">
         <v>1281</v>
       </c>
-      <c r="AP2" s="107" t="s">
+      <c r="AP2" s="104" t="s">
         <v>531</v>
       </c>
       <c r="AQ2" s="89" t="s">
         <v>217</v>
       </c>
-      <c r="AR2" s="107" t="s">
+      <c r="AR2" s="104" t="s">
         <v>1303</v>
       </c>
-      <c r="AS2" s="107" t="s">
+      <c r="AS2" s="104" t="s">
         <v>1300</v>
       </c>
       <c r="AT2" s="89" t="s">
@@ -12152,13 +12173,13 @@
       <c r="AX2" s="89" t="s">
         <v>763</v>
       </c>
-      <c r="AY2" s="105" t="s">
+      <c r="AY2" s="103" t="s">
         <v>1296</v>
       </c>
       <c r="AZ2" s="89" t="s">
         <v>1290</v>
       </c>
-      <c r="BA2" s="105" t="s">
+      <c r="BA2" s="103" t="s">
         <v>1297</v>
       </c>
       <c r="BB2" s="89">
@@ -12293,19 +12314,19 @@
       <c r="CS2" s="89" t="s">
         <v>1291</v>
       </c>
-      <c r="CT2" s="103" t="s">
+      <c r="CT2" s="102" t="s">
         <v>1206</v>
       </c>
-      <c r="CU2" s="104" t="s">
-        <v>1207</v>
-      </c>
-      <c r="CV2" s="107" t="s">
+      <c r="CU2" s="110" t="s">
+        <v>1314</v>
+      </c>
+      <c r="CV2" s="104" t="s">
         <v>1306</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="CT2" r:id="rId5" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{745B4174-B336-4C11-919C-9420C7C522AE}"/>
+    <hyperlink ref="CT2" r:id="rId4" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{745B4174-B336-4C11-919C-9420C7C522AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -12317,7 +12338,7 @@
   <dimension ref="A1:CT2"/>
   <sheetViews>
     <sheetView topLeftCell="CK1" workbookViewId="0">
-      <selection activeCell="CO19" sqref="CO19"/>
+      <selection activeCell="CS2" sqref="CS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12412,303 +12433,303 @@
     <col min="99" max="16384" style="62" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="89" customFormat="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:98" s="105" customFormat="1">
+      <c r="A1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="105" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="105" t="s">
         <v>621</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="105" t="s">
         <v>622</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="105" t="s">
         <v>623</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="105" t="s">
         <v>624</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="105" t="s">
         <v>625</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="N1" s="89" t="s">
+      <c r="N1" s="105" t="s">
         <v>238</v>
       </c>
-      <c r="O1" s="89" t="s">
+      <c r="O1" s="105" t="s">
         <v>653</v>
       </c>
-      <c r="P1" s="89" t="s">
+      <c r="P1" s="105" t="s">
         <v>654</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="105" t="s">
         <v>655</v>
       </c>
-      <c r="R1" s="89" t="s">
+      <c r="R1" s="105" t="s">
         <v>656</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="89" t="s">
+      <c r="T1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="V1" s="89" t="s">
+      <c r="V1" s="105" t="s">
         <v>1199</v>
       </c>
-      <c r="W1" s="89" t="s">
+      <c r="W1" s="105" t="s">
         <v>1209</v>
       </c>
-      <c r="X1" s="89" t="s">
+      <c r="X1" s="105" t="s">
         <v>1210</v>
       </c>
-      <c r="Y1" s="89" t="s">
+      <c r="Y1" s="105" t="s">
         <v>1211</v>
       </c>
-      <c r="Z1" s="89" t="s">
+      <c r="Z1" s="105" t="s">
         <v>796</v>
       </c>
-      <c r="AA1" s="89" t="s">
+      <c r="AA1" s="105" t="s">
         <v>1212</v>
       </c>
-      <c r="AB1" s="89" t="s">
+      <c r="AB1" s="105" t="s">
         <v>1213</v>
       </c>
-      <c r="AC1" s="89" t="s">
+      <c r="AC1" s="105" t="s">
         <v>1214</v>
       </c>
-      <c r="AD1" s="89" t="s">
+      <c r="AD1" s="105" t="s">
         <v>1215</v>
       </c>
-      <c r="AE1" s="89" t="s">
+      <c r="AE1" s="105" t="s">
         <v>1216</v>
       </c>
-      <c r="AF1" s="89" t="s">
+      <c r="AF1" s="105" t="s">
         <v>1217</v>
       </c>
-      <c r="AG1" s="89" t="s">
+      <c r="AG1" s="105" t="s">
         <v>1218</v>
       </c>
-      <c r="AH1" s="89" t="s">
+      <c r="AH1" s="105" t="s">
         <v>1219</v>
       </c>
-      <c r="AI1" s="89" t="s">
+      <c r="AI1" s="105" t="s">
         <v>1220</v>
       </c>
-      <c r="AJ1" s="89" t="s">
+      <c r="AJ1" s="105" t="s">
         <v>1221</v>
       </c>
-      <c r="AK1" s="89" t="s">
+      <c r="AK1" s="105" t="s">
         <v>1222</v>
       </c>
       <c r="AL1" s="106" t="s">
         <v>1299</v>
       </c>
-      <c r="AM1" s="89" t="s">
+      <c r="AM1" s="105" t="s">
         <v>1223</v>
       </c>
-      <c r="AN1" s="89" t="s">
+      <c r="AN1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="AO1" s="89" t="s">
+      <c r="AO1" s="105" t="s">
         <v>1224</v>
       </c>
-      <c r="AP1" s="89" t="s">
+      <c r="AP1" s="105" t="s">
         <v>1302</v>
       </c>
-      <c r="AQ1" s="89" t="s">
+      <c r="AQ1" s="105" t="s">
         <v>479</v>
       </c>
-      <c r="AR1" s="89" t="s">
+      <c r="AR1" s="105" t="s">
         <v>1225</v>
       </c>
-      <c r="AS1" s="89" t="s">
+      <c r="AS1" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="AT1" s="89" t="s">
+      <c r="AT1" s="105" t="s">
         <v>1304</v>
       </c>
-      <c r="AU1" s="89" t="s">
+      <c r="AU1" s="105" t="s">
         <v>1227</v>
       </c>
-      <c r="AV1" s="89" t="s">
+      <c r="AV1" s="105" t="s">
         <v>1228</v>
       </c>
-      <c r="AW1" s="89" t="s">
+      <c r="AW1" s="105" t="s">
         <v>1229</v>
       </c>
-      <c r="AX1" s="89" t="s">
+      <c r="AX1" s="105" t="s">
         <v>1230</v>
       </c>
-      <c r="AY1" s="89" t="s">
+      <c r="AY1" s="105" t="s">
         <v>1231</v>
       </c>
-      <c r="AZ1" s="89" t="s">
+      <c r="AZ1" s="105" t="s">
         <v>1232</v>
       </c>
-      <c r="BA1" s="89" t="s">
+      <c r="BA1" s="105" t="s">
         <v>1233</v>
       </c>
-      <c r="BB1" s="89" t="s">
+      <c r="BB1" s="105" t="s">
         <v>1234</v>
       </c>
-      <c r="BC1" s="89" t="s">
+      <c r="BC1" s="105" t="s">
         <v>1235</v>
       </c>
-      <c r="BD1" s="89" t="s">
+      <c r="BD1" s="105" t="s">
         <v>1236</v>
       </c>
-      <c r="BE1" s="89" t="s">
+      <c r="BE1" s="105" t="s">
         <v>1237</v>
       </c>
-      <c r="BF1" s="89" t="s">
+      <c r="BF1" s="105" t="s">
         <v>1238</v>
       </c>
-      <c r="BG1" s="89" t="s">
+      <c r="BG1" s="105" t="s">
         <v>1239</v>
       </c>
-      <c r="BH1" s="89" t="s">
+      <c r="BH1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BI1" s="89" t="s">
+      <c r="BI1" s="105" t="s">
         <v>1241</v>
       </c>
-      <c r="BJ1" s="89" t="s">
+      <c r="BJ1" s="105" t="s">
         <v>1242</v>
       </c>
-      <c r="BK1" s="89" t="s">
+      <c r="BK1" s="105" t="s">
         <v>1243</v>
       </c>
-      <c r="BL1" s="89" t="s">
+      <c r="BL1" s="105" t="s">
         <v>1244</v>
       </c>
-      <c r="BM1" s="89" t="s">
+      <c r="BM1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BN1" s="89" t="s">
+      <c r="BN1" s="105" t="s">
         <v>1245</v>
       </c>
-      <c r="BO1" s="89" t="s">
+      <c r="BO1" s="105" t="s">
         <v>1246</v>
       </c>
-      <c r="BP1" s="89" t="s">
+      <c r="BP1" s="105" t="s">
         <v>1247</v>
       </c>
-      <c r="BQ1" s="89" t="s">
+      <c r="BQ1" s="105" t="s">
         <v>1248</v>
       </c>
-      <c r="BR1" s="89" t="s">
+      <c r="BR1" s="105" t="s">
         <v>1249</v>
       </c>
-      <c r="BS1" s="89" t="s">
+      <c r="BS1" s="105" t="s">
         <v>1250</v>
       </c>
-      <c r="BT1" s="89" t="s">
+      <c r="BT1" s="105" t="s">
         <v>1251</v>
       </c>
-      <c r="BU1" s="89" t="s">
+      <c r="BU1" s="105" t="s">
         <v>1252</v>
       </c>
-      <c r="BV1" s="89" t="s">
+      <c r="BV1" s="105" t="s">
         <v>1253</v>
       </c>
-      <c r="BW1" s="89" t="s">
+      <c r="BW1" s="105" t="s">
         <v>1254</v>
       </c>
-      <c r="BX1" s="89" t="s">
+      <c r="BX1" s="105" t="s">
         <v>1255</v>
       </c>
-      <c r="BY1" s="89" t="s">
+      <c r="BY1" s="105" t="s">
         <v>1256</v>
       </c>
-      <c r="BZ1" s="89" t="s">
+      <c r="BZ1" s="105" t="s">
         <v>1257</v>
       </c>
-      <c r="CA1" s="89" t="s">
+      <c r="CA1" s="105" t="s">
         <v>1258</v>
       </c>
-      <c r="CB1" s="89" t="s">
+      <c r="CB1" s="105" t="s">
         <v>1259</v>
       </c>
-      <c r="CC1" s="89" t="s">
+      <c r="CC1" s="105" t="s">
         <v>1260</v>
       </c>
-      <c r="CD1" s="89" t="s">
+      <c r="CD1" s="105" t="s">
         <v>1310</v>
       </c>
-      <c r="CE1" s="89" t="s">
+      <c r="CE1" s="105" t="s">
         <v>1262</v>
       </c>
-      <c r="CF1" s="89" t="s">
+      <c r="CF1" s="105" t="s">
         <v>1263</v>
       </c>
-      <c r="CG1" s="89" t="s">
+      <c r="CG1" s="105" t="s">
         <v>1264</v>
       </c>
-      <c r="CH1" s="89" t="s">
+      <c r="CH1" s="105" t="s">
         <v>1265</v>
       </c>
-      <c r="CI1" s="89" t="s">
+      <c r="CI1" s="105" t="s">
         <v>1266</v>
       </c>
-      <c r="CJ1" s="89" t="s">
+      <c r="CJ1" s="105" t="s">
         <v>1267</v>
       </c>
-      <c r="CK1" s="89" t="s">
+      <c r="CK1" s="105" t="s">
         <v>1268</v>
       </c>
-      <c r="CL1" s="89" t="s">
+      <c r="CL1" s="105" t="s">
         <v>1269</v>
       </c>
-      <c r="CM1" s="89" t="s">
+      <c r="CM1" s="105" t="s">
         <v>1270</v>
       </c>
-      <c r="CN1" s="89" t="s">
+      <c r="CN1" s="105" t="s">
         <v>1271</v>
       </c>
-      <c r="CO1" s="89" t="s">
+      <c r="CO1" s="105" t="s">
         <v>1272</v>
       </c>
-      <c r="CP1" s="89" t="s">
+      <c r="CP1" s="105" t="s">
         <v>1273</v>
       </c>
-      <c r="CQ1" s="89" t="s">
+      <c r="CQ1" s="105" t="s">
         <v>1274</v>
       </c>
-      <c r="CR1" s="102" t="s">
+      <c r="CR1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="CS1" s="102" t="s">
+      <c r="CS1" s="105" t="s">
         <v>1199</v>
       </c>
-      <c r="CT1" s="89" t="s">
+      <c r="CT1" s="105" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="2" spans="1:98" s="89" customFormat="1">
+    <row r="2" spans="1:98" s="89" customFormat="1" ht="16.5">
       <c r="A2" s="89" t="s">
         <v>21</v>
       </c>
@@ -12853,13 +12874,13 @@
       <c r="AV2" s="89" t="s">
         <v>763</v>
       </c>
-      <c r="AW2" s="105" t="s">
+      <c r="AW2" s="103" t="s">
         <v>1296</v>
       </c>
       <c r="AX2" s="89" t="s">
         <v>1290</v>
       </c>
-      <c r="AY2" s="105" t="s">
+      <c r="AY2" s="103" t="s">
         <v>1297</v>
       </c>
       <c r="AZ2" s="89">
@@ -12994,11 +13015,11 @@
       <c r="CQ2" s="89" t="s">
         <v>1291</v>
       </c>
-      <c r="CR2" s="103" t="s">
+      <c r="CR2" s="102" t="s">
         <v>1206</v>
       </c>
-      <c r="CS2" s="104" t="s">
-        <v>1207</v>
+      <c r="CS2" s="110" t="s">
+        <v>1314</v>
       </c>
       <c r="CT2" s="56" t="s">
         <v>1306</v>
@@ -13006,7 +13027,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="CR2" r:id="rId5" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{0248B67F-86DE-493B-89DA-79462969C728}"/>
+    <hyperlink ref="CR2" r:id="rId4" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{0248B67F-86DE-493B-89DA-79462969C728}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -13015,10 +13036,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7E045B-6100-4829-941D-4D73F9115466}">
-  <dimension ref="A1:CT2"/>
+  <dimension ref="A1:CV4"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="CK1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="CT2" sqref="CT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13065,7 +13086,7 @@
     <col min="41" max="41" bestFit="true" customWidth="true" style="62" width="11.0" collapsed="true"/>
     <col min="42" max="42" style="62" width="9.140625" collapsed="true"/>
     <col min="43" max="43" bestFit="true" customWidth="true" style="62" width="13.5703125" collapsed="true"/>
-    <col min="44" max="44" style="62" width="9.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="62" width="16.42578125" collapsed="true"/>
     <col min="45" max="45" bestFit="true" customWidth="true" style="62" width="12.85546875" collapsed="true"/>
     <col min="46" max="46" bestFit="true" customWidth="true" style="62" width="18.140625" collapsed="true"/>
     <col min="47" max="47" bestFit="true" customWidth="true" style="62" width="13.42578125" collapsed="true"/>
@@ -13109,307 +13130,307 @@
     <col min="95" max="95" bestFit="true" customWidth="true" style="62" width="24.140625" collapsed="true"/>
     <col min="96" max="96" bestFit="true" customWidth="true" style="62" width="13.85546875" collapsed="true"/>
     <col min="97" max="97" bestFit="true" customWidth="true" style="62" width="32.140625" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" style="62" width="11.5703125" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" style="62" width="15.7109375" collapsed="true"/>
     <col min="99" max="16384" style="62" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="89" customFormat="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:100" s="105" customFormat="1">
+      <c r="A1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="105" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="105" t="s">
         <v>621</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="105" t="s">
         <v>622</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="105" t="s">
         <v>623</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="105" t="s">
         <v>1305</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="105" t="s">
         <v>624</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="105" t="s">
         <v>625</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="N1" s="89" t="s">
+      <c r="N1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="O1" s="89" t="s">
+      <c r="O1" s="105" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="89" t="s">
+      <c r="P1" s="105" t="s">
         <v>653</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="105" t="s">
         <v>654</v>
       </c>
-      <c r="R1" s="89" t="s">
+      <c r="R1" s="105" t="s">
         <v>655</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="105" t="s">
         <v>656</v>
       </c>
-      <c r="T1" s="89" t="s">
+      <c r="T1" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="89" t="s">
+      <c r="V1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="W1" s="89" t="s">
+      <c r="W1" s="105" t="s">
         <v>1199</v>
       </c>
-      <c r="X1" s="89" t="s">
+      <c r="X1" s="105" t="s">
         <v>1309</v>
       </c>
-      <c r="Y1" s="89" t="s">
+      <c r="Y1" s="105" t="s">
         <v>1210</v>
       </c>
-      <c r="Z1" s="89" t="s">
+      <c r="Z1" s="105" t="s">
         <v>1211</v>
       </c>
-      <c r="AA1" s="89" t="s">
+      <c r="AA1" s="105" t="s">
         <v>796</v>
       </c>
-      <c r="AB1" s="89" t="s">
+      <c r="AB1" s="105" t="s">
         <v>1212</v>
       </c>
-      <c r="AC1" s="89" t="s">
+      <c r="AC1" s="105" t="s">
         <v>1213</v>
       </c>
-      <c r="AD1" s="89" t="s">
+      <c r="AD1" s="105" t="s">
         <v>1214</v>
       </c>
-      <c r="AE1" s="89" t="s">
+      <c r="AE1" s="105" t="s">
         <v>1215</v>
       </c>
-      <c r="AF1" s="89" t="s">
+      <c r="AF1" s="105" t="s">
         <v>1216</v>
       </c>
-      <c r="AG1" s="89" t="s">
+      <c r="AG1" s="105" t="s">
         <v>1217</v>
       </c>
-      <c r="AH1" s="89" t="s">
+      <c r="AH1" s="105" t="s">
         <v>1218</v>
       </c>
-      <c r="AI1" s="89" t="s">
+      <c r="AI1" s="105" t="s">
         <v>1219</v>
       </c>
-      <c r="AJ1" s="89" t="s">
+      <c r="AJ1" s="105" t="s">
         <v>1220</v>
       </c>
-      <c r="AK1" s="89" t="s">
+      <c r="AK1" s="105" t="s">
         <v>1221</v>
       </c>
-      <c r="AL1" s="89" t="s">
+      <c r="AL1" s="105" t="s">
         <v>1222</v>
       </c>
       <c r="AM1" s="106" t="s">
         <v>1299</v>
       </c>
-      <c r="AN1" s="89" t="s">
+      <c r="AN1" s="105" t="s">
         <v>1223</v>
       </c>
-      <c r="AO1" s="89" t="s">
+      <c r="AO1" s="105" t="s">
         <v>652</v>
       </c>
-      <c r="AP1" s="89" t="s">
+      <c r="AP1" s="105" t="s">
         <v>1224</v>
       </c>
-      <c r="AQ1" s="89" t="s">
+      <c r="AQ1" s="105" t="s">
         <v>1302</v>
       </c>
-      <c r="AR1" s="89" t="s">
+      <c r="AR1" s="105" t="s">
         <v>479</v>
       </c>
-      <c r="AS1" s="89" t="s">
+      <c r="AS1" s="105" t="s">
         <v>1225</v>
       </c>
-      <c r="AT1" s="89" t="s">
+      <c r="AT1" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="AU1" s="89" t="s">
+      <c r="AU1" s="105" t="s">
         <v>1304</v>
       </c>
-      <c r="AV1" s="89" t="s">
+      <c r="AV1" s="105" t="s">
         <v>1227</v>
       </c>
-      <c r="AW1" s="89" t="s">
+      <c r="AW1" s="105" t="s">
         <v>1228</v>
       </c>
-      <c r="AX1" s="89" t="s">
+      <c r="AX1" s="105" t="s">
         <v>1229</v>
       </c>
-      <c r="AY1" s="89" t="s">
+      <c r="AY1" s="105" t="s">
         <v>1230</v>
       </c>
-      <c r="AZ1" s="89" t="s">
+      <c r="AZ1" s="105" t="s">
         <v>1231</v>
       </c>
-      <c r="BA1" s="89" t="s">
+      <c r="BA1" s="105" t="s">
         <v>1232</v>
       </c>
-      <c r="BB1" s="89" t="s">
+      <c r="BB1" s="105" t="s">
         <v>1233</v>
       </c>
-      <c r="BC1" s="89" t="s">
+      <c r="BC1" s="105" t="s">
         <v>1234</v>
       </c>
-      <c r="BD1" s="89" t="s">
+      <c r="BD1" s="105" t="s">
         <v>1235</v>
       </c>
-      <c r="BE1" s="89" t="s">
+      <c r="BE1" s="105" t="s">
         <v>1236</v>
       </c>
-      <c r="BF1" s="89" t="s">
+      <c r="BF1" s="105" t="s">
         <v>1237</v>
       </c>
-      <c r="BG1" s="89" t="s">
+      <c r="BG1" s="105" t="s">
         <v>1238</v>
       </c>
-      <c r="BH1" s="89" t="s">
+      <c r="BH1" s="105" t="s">
         <v>1239</v>
       </c>
-      <c r="BI1" s="89" t="s">
+      <c r="BI1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BJ1" s="89" t="s">
+      <c r="BJ1" s="105" t="s">
         <v>1241</v>
       </c>
-      <c r="BK1" s="89" t="s">
+      <c r="BK1" s="105" t="s">
         <v>1242</v>
       </c>
-      <c r="BL1" s="89" t="s">
+      <c r="BL1" s="105" t="s">
         <v>1243</v>
       </c>
-      <c r="BM1" s="89" t="s">
+      <c r="BM1" s="105" t="s">
         <v>1244</v>
       </c>
-      <c r="BN1" s="89" t="s">
+      <c r="BN1" s="105" t="s">
         <v>1240</v>
       </c>
-      <c r="BO1" s="89" t="s">
+      <c r="BO1" s="105" t="s">
         <v>1245</v>
       </c>
-      <c r="BP1" s="89" t="s">
+      <c r="BP1" s="105" t="s">
         <v>1246</v>
       </c>
-      <c r="BQ1" s="89" t="s">
+      <c r="BQ1" s="105" t="s">
         <v>1247</v>
       </c>
-      <c r="BR1" s="89" t="s">
+      <c r="BR1" s="105" t="s">
         <v>1248</v>
       </c>
-      <c r="BS1" s="89" t="s">
+      <c r="BS1" s="105" t="s">
         <v>1249</v>
       </c>
-      <c r="BT1" s="89" t="s">
+      <c r="BT1" s="105" t="s">
         <v>1250</v>
       </c>
-      <c r="BU1" s="89" t="s">
+      <c r="BU1" s="105" t="s">
         <v>1251</v>
       </c>
-      <c r="BV1" s="89" t="s">
+      <c r="BV1" s="105" t="s">
         <v>1252</v>
       </c>
-      <c r="BW1" s="89" t="s">
+      <c r="BW1" s="105" t="s">
         <v>1253</v>
       </c>
-      <c r="BX1" s="89" t="s">
+      <c r="BX1" s="105" t="s">
         <v>1254</v>
       </c>
-      <c r="BY1" s="89" t="s">
+      <c r="BY1" s="105" t="s">
         <v>1255</v>
       </c>
-      <c r="BZ1" s="89" t="s">
+      <c r="BZ1" s="105" t="s">
         <v>1307</v>
       </c>
-      <c r="CA1" s="89" t="s">
+      <c r="CA1" s="105" t="s">
         <v>1257</v>
       </c>
-      <c r="CB1" s="89" t="s">
+      <c r="CB1" s="105" t="s">
         <v>1258</v>
       </c>
-      <c r="CC1" s="89" t="s">
+      <c r="CC1" s="105" t="s">
         <v>1259</v>
       </c>
-      <c r="CD1" s="89" t="s">
+      <c r="CD1" s="105" t="s">
         <v>1260</v>
       </c>
-      <c r="CE1" s="89" t="s">
+      <c r="CE1" s="105" t="s">
         <v>1261</v>
       </c>
-      <c r="CF1" s="89" t="s">
+      <c r="CF1" s="105" t="s">
         <v>1262</v>
       </c>
-      <c r="CG1" s="89" t="s">
+      <c r="CG1" s="105" t="s">
         <v>1263</v>
       </c>
-      <c r="CH1" s="89" t="s">
+      <c r="CH1" s="105" t="s">
         <v>1264</v>
       </c>
-      <c r="CI1" s="89" t="s">
+      <c r="CI1" s="105" t="s">
         <v>1265</v>
       </c>
-      <c r="CJ1" s="89" t="s">
+      <c r="CJ1" s="105" t="s">
         <v>1266</v>
       </c>
-      <c r="CK1" s="89" t="s">
+      <c r="CK1" s="105" t="s">
         <v>1267</v>
       </c>
-      <c r="CL1" s="89" t="s">
+      <c r="CL1" s="105" t="s">
         <v>1268</v>
       </c>
-      <c r="CM1" s="89" t="s">
+      <c r="CM1" s="105" t="s">
         <v>1269</v>
       </c>
-      <c r="CN1" s="89" t="s">
+      <c r="CN1" s="105" t="s">
         <v>1270</v>
       </c>
-      <c r="CO1" s="89" t="s">
+      <c r="CO1" s="105" t="s">
         <v>1271</v>
       </c>
-      <c r="CP1" s="89" t="s">
+      <c r="CP1" s="105" t="s">
         <v>1272</v>
       </c>
-      <c r="CQ1" s="89" t="s">
+      <c r="CQ1" s="105" t="s">
         <v>1273</v>
       </c>
-      <c r="CR1" s="89" t="s">
+      <c r="CR1" s="105" t="s">
         <v>1274</v>
       </c>
-      <c r="CS1" s="102" t="s">
+      <c r="CS1" s="105" t="s">
         <v>1198</v>
       </c>
-      <c r="CT1" s="102" t="s">
+      <c r="CT1" s="105" t="s">
         <v>1199</v>
       </c>
     </row>
-    <row r="2" spans="1:98" s="89" customFormat="1">
+    <row r="2" spans="1:100" s="89" customFormat="1" ht="16.5">
       <c r="A2" s="89" t="s">
         <v>21</v>
       </c>
@@ -13428,8 +13449,8 @@
       <c r="F2" s="89">
         <v>9988776655</v>
       </c>
-      <c r="G2" s="107" t="s">
-        <v>1306</v>
+      <c r="G2" s="56" t="s">
+        <v>1313</v>
       </c>
       <c r="H2" s="89">
         <v>9988</v>
@@ -13530,17 +13551,17 @@
       <c r="AN2" s="89" t="s">
         <v>1281</v>
       </c>
-      <c r="AO2" s="107" t="s">
+      <c r="AO2" s="104" t="s">
         <v>531</v>
       </c>
       <c r="AP2" s="89" t="s">
         <v>217</v>
       </c>
-      <c r="AQ2" s="107" t="s">
+      <c r="AQ2" s="104" t="s">
         <v>1303</v>
       </c>
-      <c r="AR2" s="107" t="s">
-        <v>1300</v>
+      <c r="AR2" s="56" t="s">
+        <v>735</v>
       </c>
       <c r="AS2" s="89" t="s">
         <v>1289</v>
@@ -13557,13 +13578,13 @@
       <c r="AW2" s="89" t="s">
         <v>763</v>
       </c>
-      <c r="AX2" s="105" t="s">
+      <c r="AX2" s="103" t="s">
         <v>1296</v>
       </c>
       <c r="AY2" s="89" t="s">
         <v>1290</v>
       </c>
-      <c r="AZ2" s="105" t="s">
+      <c r="AZ2" s="103" t="s">
         <v>1297</v>
       </c>
       <c r="BA2" s="89">
@@ -13641,7 +13662,7 @@
       <c r="BY2" s="89" t="s">
         <v>1292</v>
       </c>
-      <c r="BZ2" s="107" t="s">
+      <c r="BZ2" s="104" t="s">
         <v>1308</v>
       </c>
       <c r="CA2" s="89" t="s">
@@ -13698,16 +13719,23 @@
       <c r="CR2" s="89" t="s">
         <v>1291</v>
       </c>
-      <c r="CS2" s="103" t="s">
+      <c r="CS2" s="102" t="s">
         <v>1206</v>
       </c>
-      <c r="CT2" s="104" t="s">
-        <v>1207</v>
-      </c>
+      <c r="CT2" s="110" t="s">
+        <v>1314</v>
+      </c>
+      <c r="CV2" s="108"/>
+    </row>
+    <row r="3" spans="1:100">
+      <c r="CT3"/>
+    </row>
+    <row r="4" spans="1:100" ht="16.5">
+      <c r="CT4" s="109"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="CS2" r:id="rId5" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{AAA75900-8D8F-464A-8AB8-0B1E11EF7673}"/>
+    <hyperlink ref="CS2" r:id="rId4" tooltip="mailto:banu.daikin@solunus.com.cpqdev" display="mailto:banu.daikin@solunus.com.cpqdev" xr:uid="{AAA75900-8D8F-464A-8AB8-0B1E11EF7673}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -13719,7 +13747,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13743,71 +13771,71 @@
     <col min="22" max="22" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="32" customFormat="1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:22" s="107" customFormat="1">
+      <c r="A1" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="107" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="107" t="s">
         <v>621</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="107" t="s">
         <v>622</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="107" t="s">
         <v>623</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="107" t="s">
         <v>624</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="107" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="107" t="s">
         <v>625</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="107" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="107" t="s">
         <v>652</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="107" t="s">
         <v>238</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="107" t="s">
         <v>653</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="107" t="s">
         <v>654</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="107" t="s">
         <v>655</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="R1" s="107" t="s">
         <v>656</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="U1" s="107" t="s">
         <v>1198</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="107" t="s">
         <v>1199</v>
       </c>
     </row>
@@ -13950,12 +13978,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId20" xr:uid="{97F4D6FC-7A82-4B45-B6FF-12B0A5638E5C}"/>
-    <hyperlink ref="U2" r:id="rId21" xr:uid="{CCA28E27-300E-471A-87E5-BDB3102195B8}"/>
-    <hyperlink ref="V2" r:id="rId22" xr:uid="{37CB7323-D2D1-4117-9120-69411C82610B}"/>
-    <hyperlink ref="C3" r:id="rId23" xr:uid="{809953F5-3104-4DFE-B885-A5D2FDA15047}"/>
-    <hyperlink ref="U3" r:id="rId24" xr:uid="{94AA6731-ADA2-4915-8B0C-BADF3A9F30A0}"/>
-    <hyperlink ref="V3" r:id="rId25" xr:uid="{D1072976-28C8-4CC7-B911-0E2BEC56DC67}"/>
+    <hyperlink ref="C2" r:id="rId14" xr:uid="{97F4D6FC-7A82-4B45-B6FF-12B0A5638E5C}"/>
+    <hyperlink ref="U2" r:id="rId15" xr:uid="{CCA28E27-300E-471A-87E5-BDB3102195B8}"/>
+    <hyperlink ref="V2" r:id="rId16" xr:uid="{37CB7323-D2D1-4117-9120-69411C82610B}"/>
+    <hyperlink ref="C3" r:id="rId17" xr:uid="{809953F5-3104-4DFE-B885-A5D2FDA15047}"/>
+    <hyperlink ref="U3" r:id="rId18" xr:uid="{94AA6731-ADA2-4915-8B0C-BADF3A9F30A0}"/>
+    <hyperlink ref="V3" r:id="rId19" xr:uid="{D1072976-28C8-4CC7-B911-0E2BEC56DC67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -14001,8 +14029,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId7" xr:uid="{1C396A09-1007-429A-87A0-C75A610DC5BD}"/>
-    <hyperlink ref="B2" r:id="rId8" xr:uid="{5485457F-C537-4F67-87DB-1638CC269A44}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{1C396A09-1007-429A-87A0-C75A610DC5BD}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{5485457F-C537-4F67-87DB-1638CC269A44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15373,8 +15401,8 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AA2" r:id="rId8" xr:uid="{2C8676F0-10B3-4F66-A917-DF5CE671B698}"/>
-    <hyperlink ref="AA3:AA5" r:id="rId9" display="xyz@gmail.com" xr:uid="{70E13282-7532-4066-AE56-7A6091E3B281}"/>
+    <hyperlink ref="AA2" r:id="rId6" xr:uid="{2C8676F0-10B3-4F66-A917-DF5CE671B698}"/>
+    <hyperlink ref="AA3:AA5" r:id="rId7" display="xyz@gmail.com" xr:uid="{70E13282-7532-4066-AE56-7A6091E3B281}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -15989,8 +16017,8 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Z2" r:id="rId7" xr:uid="{C6D004E2-4F87-4173-99C2-A7B382C07D1B}"/>
-    <hyperlink ref="Z3:Z5" r:id="rId8" display="test@gmail.com" xr:uid="{EB559366-D2E2-4016-B76E-FD56AF7AD0D6}"/>
+    <hyperlink ref="Z2" r:id="rId5" xr:uid="{C6D004E2-4F87-4173-99C2-A7B382C07D1B}"/>
+    <hyperlink ref="Z3:Z5" r:id="rId6" display="test@gmail.com" xr:uid="{EB559366-D2E2-4016-B76E-FD56AF7AD0D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>